<commit_message>
Attenuation added to point light
</commit_message>
<xml_diff>
--- a/Documents/Dev IV Solo Project Rubric.xlsx
+++ b/Documents/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8334C2F3-FF38-47BB-8796-FE9CCB219DBB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A37CE0-0F50-476E-B140-FCB7F373D56C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,15 +1048,19 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G67" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1072,7 +1076,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1088,11 +1092,15 @@
       <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>26</v>
@@ -1158,11 +1166,15 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>22</v>
@@ -1197,7 +1209,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>

</xml_diff>

<commit_message>
Added zoom on ctrl/ctrl+lshift
</commit_message>
<xml_diff>
--- a/Documents/Dev IV Solo Project Rubric.xlsx
+++ b/Documents/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A37CE0-0F50-476E-B140-FCB7F373D56C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA74A52E-21F1-4A5C-A9E4-E3B3176E5D93}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1201,15 +1201,19 @@
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
@@ -1235,11 +1239,15 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>25</v>
@@ -2503,11 +2511,15 @@
       <c r="D64" s="5">
         <v>1</v>
       </c>
-      <c r="E64" s="2"/>
-      <c r="F64" s="3"/>
+      <c r="E64" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G64" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
@@ -3240,7 +3252,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Camera working on Translation-WASD Rotation-IJKL
</commit_message>
<xml_diff>
--- a/Documents/Dev IV Solo Project Rubric.xlsx
+++ b/Documents/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA74A52E-21F1-4A5C-A9E4-E3B3176E5D93}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1A9245-F700-4541-B29B-7F76A036327F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -933,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1067,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1076,7 +1079,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1217,7 +1220,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
@@ -2486,11 +2489,15 @@
       <c r="D63" s="5">
         <v>2</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="3"/>
+      <c r="E63" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
@@ -3252,7 +3259,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Per-Pixel lighting implemented, Black and White toggle on '4'
</commit_message>
<xml_diff>
--- a/Documents/Dev IV Solo Project Rubric.xlsx
+++ b/Documents/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1A9245-F700-4541-B29B-7F76A036327F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA1014F-B72C-4D77-963E-0E426C424AC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1132,11 +1132,15 @@
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
@@ -1220,7 +1224,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
@@ -1277,11 +1281,15 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
@@ -1411,11 +1419,15 @@
       <c r="D15" s="5">
         <v>2</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
+      <c r="E15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -3259,7 +3271,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
New vertex shader using sine wave
</commit_message>
<xml_diff>
--- a/Documents/Dev IV Solo Project Rubric.xlsx
+++ b/Documents/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA1014F-B72C-4D77-963E-0E426C424AC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328C0DB3-583C-45EE-A342-5461066F225D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,11 +1063,11 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1220,11 +1220,11 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
@@ -2134,11 +2134,15 @@
       <c r="D46" s="5">
         <v>2</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="3"/>
+      <c r="E46" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G46" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -2531,7 +2535,7 @@
         <v>1</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>103</v>
@@ -2737,11 +2741,15 @@
       <c r="D73" s="5">
         <v>1</v>
       </c>
-      <c r="E73" s="2"/>
-      <c r="F73" s="3"/>
+      <c r="E73" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G73" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>

</xml_diff>

<commit_message>
Added wave format to new pixel shader to simulate clouds (toggle through Pixel shaders with '4')
</commit_message>
<xml_diff>
--- a/Documents/Dev IV Solo Project Rubric.xlsx
+++ b/Documents/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328C0DB3-583C-45EE-A342-5461066F225D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7096E8E-44E3-481E-BC5F-AB7C028482EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,11 +1063,11 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1075,11 +1075,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
@@ -1220,15 +1220,15 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1293,11 +1293,11 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -1702,11 +1702,15 @@
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
+      <c r="E28" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -3126,8 +3130,12 @@
       <c r="B91" s="6">
         <v>2</v>
       </c>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
+      <c r="C91" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -3144,8 +3152,12 @@
       <c r="B92" s="6">
         <v>1</v>
       </c>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
+      <c r="C92" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="E92" s="3"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
@@ -3279,7 +3291,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Camera and aspect ratio saved when window is resized
</commit_message>
<xml_diff>
--- a/Documents/Dev IV Solo Project Rubric.xlsx
+++ b/Documents/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F613903F-6764-4FD9-AFDA-7A7D2BA16854}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02101110-4C56-448D-B1D6-7CC7580372CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,11 +1075,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1293,11 +1293,11 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -2381,11 +2381,15 @@
       <c r="D57" s="5">
         <v>2</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="3"/>
+      <c r="E57" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -3295,7 +3299,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Updated excel file for grading Controls: WASD - translate camera x/z space/shift-space - translate camera y IJKL - rotate camera arrow keys - modify near and far plane ctrl/shift-ctrl - change fov (zoom camera) '1' - toggle directional light '2' - toggle point light '3' - toggle spot light '4' - toggle through pixel shaders (black and white & sine wave) '5' - toggle vertex shaders (sine wave)
</commit_message>
<xml_diff>
--- a/Documents/Dev IV Solo Project Rubric.xlsx
+++ b/Documents/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02101110-4C56-448D-B1D6-7CC7580372CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987DA756-765F-44F7-B5DD-C803B35FDD3A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,11 +1075,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1293,11 +1293,11 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -1616,11 +1616,15 @@
       <c r="D24" s="5">
         <v>3</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G24" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -3299,7 +3303,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Fixing issue with pushing (commited large files)
</commit_message>
<xml_diff>
--- a/Documents/Dev IV Solo Project Rubric.xlsx
+++ b/Documents/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987DA756-765F-44F7-B5DD-C803B35FDD3A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DD04AF-A734-4482-8E72-4C564D0E1A80}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/3d-models/medieval-fantasy-book-06d5a80a04fc4c5ab552759e9a97d91a</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -936,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1077,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1079,7 +1085,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1228,7 +1234,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1967,11 +1973,15 @@
       <c r="D39" s="5">
         <v>4</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="3"/>
+      <c r="E39" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G39" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -3213,7 +3223,9 @@
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" s="12"/>
+      <c r="A96" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
@@ -3303,7 +3315,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added Dwarf and Wizard to scene, using IndexedInstance on dwarf
</commit_message>
<xml_diff>
--- a/Documents/Dev IV Solo Project Rubric.xlsx
+++ b/Documents/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF99C7D-351A-4A85-8401-DFDD692C0266}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06736C0E-CE09-4C91-A109-46D8B0E72A17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="109">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>https://sketchfab.com/3d-models/black-dragon-with-idle-animation-fb0053a2e59b43868e934c239bf4eb36</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/3d-models/the-dwarf-16a5f56515304e16899960b6a17b88f1</t>
   </si>
 </sst>
 </file>
@@ -945,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,15 +1083,15 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1157,7 +1160,7 @@
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
@@ -1237,7 +1240,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1302,11 +1305,11 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -1429,7 +1432,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>103</v>
@@ -2005,11 +2008,15 @@
       <c r="D40" s="5">
         <v>3</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G40" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -2973,11 +2980,15 @@
       <c r="D82" s="5">
         <v>3</v>
       </c>
-      <c r="E82" s="2"/>
-      <c r="F82" s="3"/>
+      <c r="E82" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G82" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
@@ -3240,7 +3251,9 @@
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="12"/>
+      <c r="A98" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
@@ -3324,7 +3337,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Reflective material through cube mapping included
</commit_message>
<xml_diff>
--- a/Documents/Dev IV Solo Project Rubric.xlsx
+++ b/Documents/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06736C0E-CE09-4C91-A109-46D8B0E72A17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D426E7C-3752-484D-A935-71344276404E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="112">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -355,6 +355,15 @@
   </si>
   <si>
     <t>https://sketchfab.com/3d-models/the-dwarf-16a5f56515304e16899960b6a17b88f1</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/3d-models/paladin-4f1c320f2cec49dc9bf38c6aad2d8ea9</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/3d-models/wizard-asset-fot-tower-of-the-wizard-scene-2bee14d9fbf649d28ba20aad3e0c6790</t>
+  </si>
+  <si>
+    <t>http://www.custommapmakers.org/skyboxes/zips/ame_limon.zip</t>
   </si>
 </sst>
 </file>
@@ -948,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1092,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1091,7 +1100,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1169,7 +1178,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 60, SUM(-60,L4),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1313,7 +1322,7 @@
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1772,11 +1781,15 @@
       <c r="D30" s="5">
         <v>2</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -3256,13 +3269,19 @@
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
+      <c r="A99" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="12"/>
+      <c r="A100" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="12"/>
+      <c r="A101" s="12" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
@@ -3337,7 +3356,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>